<commit_message>
add test case 13-16
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/user.xlsx
+++ b/src/test/resources/testdata/user.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Email</t>
   </si>
@@ -32,16 +32,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>nhl10@gmail.com</t>
-  </si>
-  <si>
     <t>nhl11@gmail.com</t>
   </si>
   <si>
     <t>nhl12@gmail.com</t>
-  </si>
-  <si>
-    <t>nhl13@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -370,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +392,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
@@ -406,27 +400,13 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>123456</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
-    <hyperlink ref="A5" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>